<commit_message>
Web App : Added add/edit/delete methods for history & dictionnary. Dictionnary visuals are still to fix
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -144,16 +144,26 @@
   </si>
   <si>
     <t>Gestion des patterns et du taux de confiance</t>
+  </si>
+  <si>
+    <t>Mise en place du login Web</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Implémentation des requêtes SQL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,8 +185,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +223,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -256,14 +278,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -273,26 +322,49 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3"/>
-    <xf numFmtId="8" fontId="2" fillId="5" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40 % - Accent4" xfId="1" builtinId="43"/>
     <cellStyle name="60 % - Accent4" xfId="2" builtinId="44"/>
+    <cellStyle name="Neutre" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="3" builtinId="26"/>
   </cellStyles>
@@ -417,7 +489,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$1:$D$2</c:f>
+              <c:f>Feuil1!$E$1:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -443,24 +515,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$3:$D$12</c:f>
+              <c:f>Feuil1!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8</c:v>
@@ -492,7 +564,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$1:$E$2</c:f>
+              <c:f>Feuil1!$F$1:$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -518,21 +590,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$3:$E$12</c:f>
+              <c:f>Feuil1!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,13 +1480,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -1446,8 +1518,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="K1:N35" totalsRowShown="0">
-  <autoFilter ref="K1:N35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="L1:O35" totalsRowShown="0">
+  <autoFilter ref="L1:O35"/>
   <tableColumns count="4">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Tasks"/>
@@ -1755,623 +1827,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="50.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="G2" s="13"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>42907</v>
+      </c>
+      <c r="B3" s="17">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8">
+      <c r="C3" s="16"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15">
+        <v>27</v>
+      </c>
+      <c r="F3" s="15">
+        <v>27</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>42908</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <f>E3-C4</f>
         <v>25</v>
       </c>
-      <c r="E3" s="8">
-        <v>25</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="K3" s="11">
+      <c r="F4" s="15">
+        <f>F3-D4</f>
+        <v>26</v>
+      </c>
+      <c r="G4" s="15">
+        <f>F3-F4</f>
         <v>1</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L4" s="5">
+        <v>2</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>42909</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15">
         <v>5</v>
       </c>
-      <c r="M3" s="11">
+      <c r="D5" s="15">
+        <v>6</v>
+      </c>
+      <c r="E5" s="15">
+        <f>E4-C5</f>
+        <v>20</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" ref="F5:F6" si="0">F4-D5</f>
+        <v>20</v>
+      </c>
+      <c r="G5" s="15">
+        <f t="shared" ref="G5:G12" si="1">F4-F5</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="5">
         <v>0.5</v>
       </c>
-      <c r="N3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="O5" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <f>D3-B4</f>
-        <v>23</v>
-      </c>
-      <c r="E4" s="8">
-        <f>E3-C4</f>
-        <v>24</v>
-      </c>
-      <c r="F4" s="8">
-        <f>E3-E4</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="11">
-        <v>2</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="N4" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>42910</v>
+      </c>
+      <c r="B6" s="17">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6</v>
+      </c>
+      <c r="D6" s="15">
         <v>5</v>
       </c>
-      <c r="C5" s="8">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8">
-        <f>D4-B5</f>
-        <v>18</v>
-      </c>
-      <c r="E5" s="8">
-        <f t="shared" ref="E5:E6" si="0">E4-C5</f>
-        <v>18</v>
-      </c>
-      <c r="F5" s="8">
-        <f t="shared" ref="F5:F12" si="1">E4-E5</f>
-        <v>6</v>
-      </c>
-      <c r="K5" s="11">
-        <v>3</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="N5" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8">
-        <v>6</v>
-      </c>
-      <c r="C6" s="8">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8">
-        <f>D5-B6</f>
-        <v>12</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="E6" s="15">
+        <f>E5-C6</f>
+        <v>14</v>
+      </c>
+      <c r="F6" s="15">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F6" s="8">
+        <v>15</v>
+      </c>
+      <c r="G6" s="15">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>4</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>7</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.5</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>42911</v>
+      </c>
+      <c r="B7" s="17">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8">
-        <f>D6-B7</f>
-        <v>11</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8">
+      <c r="C7" s="15">
+        <v>2</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15">
+        <f>E6-C7</f>
+        <v>12</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="K7">
+        <v>15</v>
+      </c>
+      <c r="L7">
         <v>5</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>9</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0.5</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>42912</v>
+      </c>
+      <c r="B8" s="18">
         <v>5</v>
       </c>
-      <c r="B8" s="8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8">
-        <f>D7-B8</f>
+      <c r="C8" s="15">
+        <v>4</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15">
+        <f>E7-C8</f>
         <v>8</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8">
+      <c r="F8" s="15"/>
+      <c r="G8" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="4"/>
       <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>42913</v>
+      </c>
+      <c r="B9" s="18">
         <v>6</v>
       </c>
-      <c r="B9" s="8">
+      <c r="C9" s="15">
         <v>3</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8">
-        <f>D8-B9</f>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15">
+        <f>E8-C9</f>
         <v>5</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8">
+      <c r="F9" s="15"/>
+      <c r="G9" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>42914</v>
+      </c>
+      <c r="B10" s="18">
         <v>7</v>
       </c>
-      <c r="B10" s="8">
+      <c r="C10" s="15">
         <v>3</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8">
-        <f t="shared" ref="D10:D12" si="2">D9-B10</f>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15">
+        <f t="shared" ref="E10:E12" si="2">E9-C10</f>
         <v>2</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8">
+      <c r="F10" s="15"/>
+      <c r="G10" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="11">
+      <c r="L10" s="5">
         <v>6</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="M10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="11">
+      <c r="N10" s="5">
         <v>2</v>
       </c>
-      <c r="N10" s="11">
+      <c r="O10" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>42915</v>
+      </c>
+      <c r="B11" s="18">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="C11" s="15">
         <v>1</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8">
+      <c r="D11" s="15"/>
+      <c r="E11" s="15">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="11">
+      <c r="L11" s="5">
         <v>7</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="M11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="11">
+      <c r="N11" s="5">
         <v>0.5</v>
       </c>
-      <c r="N11" s="11">
+      <c r="O11" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>42916</v>
+      </c>
+      <c r="B12" s="18">
         <v>9</v>
       </c>
-      <c r="B12" s="8">
+      <c r="C12" s="15">
         <v>1</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K12" s="11">
+      <c r="L12" s="5">
         <v>8</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="M12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="11">
+      <c r="N12" s="5">
         <v>2</v>
       </c>
-      <c r="N12" s="11">
+      <c r="O12" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K13">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L13">
         <v>9</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>15</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>0.5</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K14">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L14">
         <v>10</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>16</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K15" s="3"/>
-      <c r="L15" s="1" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L15" s="3"/>
+      <c r="M15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K16" s="11">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L16" s="5">
         <v>11</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="M16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M16" s="11">
+      <c r="N16" s="5">
         <v>1</v>
       </c>
-      <c r="N16" s="11">
+      <c r="O16" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K17" s="11">
+    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L17" s="5">
         <v>12</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="M17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="11">
+      <c r="N17" s="5">
         <v>1</v>
       </c>
-      <c r="N17" s="11">
+      <c r="O17" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K18">
+    <row r="18" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L18">
         <v>13</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>20</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>3</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K19">
+    <row r="19" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L19">
         <v>14</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>21</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>2</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K20">
+    <row r="20" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L20">
         <v>15</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>34</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>2</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K21">
+    <row r="21" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L21">
         <v>16</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>35</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>2</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K23" s="4"/>
-      <c r="L23" s="2" t="s">
+    <row r="23" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L23" s="4"/>
+      <c r="M23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="4"/>
       <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K24">
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L24">
         <v>17</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>23</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>2</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K25">
+    <row r="25" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L25">
         <v>18</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>24</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>3</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K26" s="11">
+    <row r="26" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="5">
         <v>19</v>
       </c>
-      <c r="L26" s="11" t="s">
+      <c r="M26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="11">
+      <c r="N26" s="5">
         <v>1</v>
       </c>
-      <c r="N26" s="11">
+      <c r="O26" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K27">
+    <row r="27" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L27">
         <v>20</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>25</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>2</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K28">
+    <row r="28" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L28">
         <v>21</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>26</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>4</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K29" s="11">
+    <row r="29" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L29" s="5">
         <v>22</v>
       </c>
-      <c r="L29" s="11" t="s">
+      <c r="M29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="11">
+      <c r="N29" s="5">
         <v>1</v>
       </c>
-      <c r="N29" s="11">
+      <c r="O29" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K30" s="11">
+    <row r="30" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L30" s="5">
         <v>23</v>
       </c>
-      <c r="L30" s="12" t="s">
+      <c r="M30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="M30" s="11">
+      <c r="N30" s="5">
         <v>1</v>
       </c>
-      <c r="N30" s="11">
+      <c r="O30" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K31" s="11">
+    <row r="31" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L31" s="5">
         <v>24</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="M31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M31" s="11">
+      <c r="N31" s="5">
         <v>1</v>
       </c>
-      <c r="N31" s="11">
+      <c r="O31" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K32">
+    <row r="32" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L32">
         <v>25</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>39</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>4</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>6</v>
       </c>
     </row>
+    <row r="33" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>26</v>
+      </c>
+      <c r="M33" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>27</v>
+      </c>
+      <c r="M34" t="s">
+        <v>42</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="5">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Gestion de projet mamène
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Desktop\Exia\A4\UE 3\Projet JEE WCF\Github projet JEE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Desktop\Exia\A4\UE 3\Projet JEE WCF\ProjetTotalementSecretANePasTransmettre\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -161,9 +161,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,8 +192,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +246,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -304,15 +327,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,26 +363,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="8" fontId="2" fillId="5" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,13 +381,33 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="40 % - Accent4" xfId="1" builtinId="43"/>
     <cellStyle name="60 % - Accent4" xfId="2" builtinId="44"/>
     <cellStyle name="Neutre" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="3" builtinId="26"/>
+    <cellStyle name="Vérification" xfId="5" builtinId="23"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -605,6 +646,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1830,7 +1880,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,21 +1891,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="17" t="s">
         <v>31</v>
       </c>
       <c r="L1" t="s">
@@ -1872,21 +1922,21 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="14" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="18"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
         <v>4</v>
@@ -1895,21 +1945,21 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>42907</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15">
+      <c r="C3" s="10"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9">
         <v>27</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="9">
         <v>27</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="9"/>
       <c r="L3" s="5">
         <v>1</v>
       </c>
@@ -1924,27 +1974,27 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>42908</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="9">
         <f>E3-C4</f>
         <v>25</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="9">
         <f>F3-D4</f>
         <v>26</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="9">
         <f>F3-F4</f>
         <v>1</v>
       </c>
@@ -1962,27 +2012,27 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>42909</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="9">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="9">
         <v>6</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="9">
         <f>E4-C5</f>
         <v>20</v>
       </c>
-      <c r="F5" s="15">
-        <f t="shared" ref="F5:F6" si="0">F4-D5</f>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5:F9" si="0">F4-D5</f>
         <v>20</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="9">
         <f t="shared" ref="G5:G12" si="1">F4-F5</f>
         <v>6</v>
       </c>
@@ -2000,95 +2050,105 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>42910</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="9">
         <v>6</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="9">
         <v>5</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="9">
         <f>E5-C6</f>
         <v>14</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="9">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>4</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <v>0.5</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>42911</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15">
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
         <f>E6-C7</f>
         <v>12</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15">
+      <c r="F7" s="9">
+        <f>F6-D7</f>
+        <v>13</v>
+      </c>
+      <c r="G7" s="9">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5">
         <v>5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <v>0.5</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>42912</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="9">
         <v>4</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15">
+      <c r="D8" s="9">
+        <v>3</v>
+      </c>
+      <c r="E8" s="9">
         <f>E7-C8</f>
         <v>8</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15">
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G8" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="2" t="s">
@@ -2098,22 +2158,25 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>42913</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="12">
         <v>6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <f>E8-C9</f>
         <v>5</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15">
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2125,58 +2188,58 @@
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>42914</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="12">
         <v>7</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="9">
         <v>3</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <f t="shared" ref="E10:E12" si="2">E9-C10</f>
         <v>2</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L10" s="5">
+        <v>6</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="5">
+        <v>2</v>
+      </c>
+      <c r="O10" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>42915</v>
+      </c>
+      <c r="B11" s="12">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="5">
-        <v>6</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="5">
-        <v>2</v>
-      </c>
-      <c r="O10" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>42915</v>
-      </c>
-      <c r="B11" s="18">
-        <v>8</v>
-      </c>
-      <c r="C11" s="15">
-        <v>1</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="L11" s="5">
         <v>7</v>
       </c>
@@ -2191,22 +2254,22 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>42916</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="12">
         <v>9</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2288,58 +2351,58 @@
       </c>
     </row>
     <row r="18" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L18">
+      <c r="L18" s="5">
         <v>13</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="5">
         <v>3</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L19">
+      <c r="L19" s="5">
         <v>14</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="5">
         <v>2</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L20">
+      <c r="L20" s="5">
         <v>15</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="5">
         <v>2</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L21">
+      <c r="L21" s="5">
         <v>16</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="5">
         <v>2</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="5">
         <v>8</v>
       </c>
     </row>
@@ -2408,16 +2471,16 @@
       </c>
     </row>
     <row r="28" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L28">
+      <c r="L28" s="5">
         <v>21</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="5">
         <v>4</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="5">
         <v>5</v>
       </c>
     </row>
@@ -2463,7 +2526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L32">
         <v>25</v>
       </c>
@@ -2477,31 +2540,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L33">
+    <row r="33" spans="12:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L33" s="19">
         <v>26</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M33" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="19">
         <v>2</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L34">
+    <row r="34" spans="12:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L34" s="5">
         <v>27</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M34" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="5">
         <v>1</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="5">
         <v>5</v>
       </c>
     </row>
@@ -2514,9 +2577,10 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>